<commit_message>
Help and Forecaster Done
</commit_message>
<xml_diff>
--- a/processedData/models.xlsx
+++ b/processedData/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Dropbox\Online Learning\Data Science\Data Science Specialization\9. Data Products\forecast\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Dropbox\Online Learning\Data Science\Data Science Specialization\9. Data Products\homalytics\processedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,6 @@
     <t>Arima</t>
   </si>
   <si>
-    <t>In statistics and econometrics, and in particular in time series analysis, an autoregressive integrated moving average (ARIMA) model is a generalization of an autoregressive moving average (ARMA) model. These models are fitted to time series data either to better understand the data or to predict future points in the series (forecasting). They are applied in some cases where data show evidence of non-stationarity, where an initial differencing step (corresponding to the "integrated" part of the model) can be applied to reduce the non-stationarity.[1]</t>
-  </si>
-  <si>
     <t>desc</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Naive</t>
+  </si>
+  <si>
+    <t>In statistics and econometrics, and in particular in time series analysis, an autoregressive integrated moving average (ARIMA) model is a generalization of an autoregressive moving average (ARMA) model. These models are fitted to time series data either to better understand the data or to predict future points in the series (forecasting). They are applied in some cases where data show evidence of non-stationarity, where an initial differencing step (corresponding to the "integrated" part of the model) can be applied to reduce the non-stationarity.</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -484,119 +484,119 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>